<commit_message>
documents @ data provider code
</commit_message>
<xml_diff>
--- a/AutoDeskFramework/testData/TestData.xlsx
+++ b/AutoDeskFramework/testData/TestData.xlsx
@@ -4,14 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="6075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="6075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
-    <sheet name="Org" sheetId="2" r:id="rId2"/>
+    <sheet name="SingUP" sheetId="3" r:id="rId2"/>
+    <sheet name="addToCart" sheetId="4" r:id="rId3"/>
+    <sheet name="addToCartTest" sheetId="5" r:id="rId4"/>
+    <sheet name="Org" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I13"/>
+  <oleSize ref="A1:O13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="131">
   <si>
     <t>TestID</t>
   </si>
@@ -90,6 +93,330 @@
   </si>
   <si>
     <t>industry</t>
+  </si>
+  <si>
+    <t>SingUP</t>
+  </si>
+  <si>
+    <t>firstNAme</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>PhoneNum</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iphone </t>
+  </si>
+  <si>
+    <t>XR-1</t>
+  </si>
+  <si>
+    <t>XR-2</t>
+  </si>
+  <si>
+    <t>XR-3</t>
+  </si>
+  <si>
+    <t>XR-4</t>
+  </si>
+  <si>
+    <t>XR-5</t>
+  </si>
+  <si>
+    <t>XR-6</t>
+  </si>
+  <si>
+    <t>XR-7</t>
+  </si>
+  <si>
+    <t>Nokia</t>
+  </si>
+  <si>
+    <t>n-1100</t>
+  </si>
+  <si>
+    <t>n-1101</t>
+  </si>
+  <si>
+    <t>n-1102</t>
+  </si>
+  <si>
+    <t>n-1103</t>
+  </si>
+  <si>
+    <t>n-1104</t>
+  </si>
+  <si>
+    <t>n-1105</t>
+  </si>
+  <si>
+    <t>n-1106</t>
+  </si>
+  <si>
+    <t>n-1107</t>
+  </si>
+  <si>
+    <t>n-1108</t>
+  </si>
+  <si>
+    <t>n-1109</t>
+  </si>
+  <si>
+    <t>n-1110</t>
+  </si>
+  <si>
+    <t>n-1111</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>A-50</t>
+  </si>
+  <si>
+    <t>A-51</t>
+  </si>
+  <si>
+    <t>A-52</t>
+  </si>
+  <si>
+    <t>A-53</t>
+  </si>
+  <si>
+    <t>A-54</t>
+  </si>
+  <si>
+    <t>A-55</t>
+  </si>
+  <si>
+    <t>A-56</t>
+  </si>
+  <si>
+    <t>A-57</t>
+  </si>
+  <si>
+    <t>A-58</t>
+  </si>
+  <si>
+    <t>A-59</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>A-60</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>A-61</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>A-62</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>A-63</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>A-64</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>A-65</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>A-66</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>A-67</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>A-68</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>A-69</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>A-70</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>A-71</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>A-72</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>A-73</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>A-74</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>A-75</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>A-76</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>A-77</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>A-78</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>A-79</t>
+  </si>
+  <si>
+    <t>49</t>
   </si>
 </sst>
 </file>
@@ -131,10 +458,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J310"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,6 +2110,1061 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C109"/>
+  <sheetViews>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="C30" sqref="A1:C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>

</xml_diff>